<commit_message>
Definition of Done Listo
</commit_message>
<xml_diff>
--- a/product_backlog_grupo_1_s3_mauricio_rojas.xlsx
+++ b/product_backlog_grupo_1_s3_mauricio_rojas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\s3 ingenieria software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B52587-C449-466A-8EA2-734AE87D3573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7007FFAB-ADB6-4088-9198-26F94677D782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -512,19 +512,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -963,8 +963,8 @@
   </sheetPr>
   <dimension ref="A1:K993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1028,7 +1028,7 @@
       <c r="D2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="16" t="s">
         <v>63</v>
       </c>
       <c r="F2" s="10">
@@ -1057,19 +1057,19 @@
       <c r="B3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="18"/>
+      <c r="E3" s="16"/>
       <c r="F3" s="10">
         <v>12</v>
       </c>
       <c r="G3" s="11">
         <v>3</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="10" t="s">
         <v>30</v>
       </c>
@@ -1084,19 +1084,19 @@
       <c r="B4" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="10">
         <v>10</v>
       </c>
       <c r="G4" s="11">
         <v>2</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="10" t="s">
         <v>30</v>
       </c>
@@ -1111,19 +1111,19 @@
       <c r="B5" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="10">
         <v>16</v>
       </c>
       <c r="G5" s="11">
         <v>4</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="10" t="s">
         <v>30</v>
       </c>
@@ -1173,19 +1173,19 @@
       <c r="B7" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="10">
         <v>18</v>
       </c>
       <c r="G7" s="11">
         <v>5</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="10" t="s">
         <v>30</v>
       </c>
@@ -1200,19 +1200,19 @@
       <c r="B8" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="10">
         <v>15</v>
       </c>
       <c r="G8" s="11">
         <v>5</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
       <c r="J8" s="10" t="s">
         <v>38</v>
       </c>
@@ -1227,7 +1227,7 @@
       <c r="B9" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -1262,19 +1262,19 @@
       <c r="B10" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="10">
         <v>20</v>
       </c>
       <c r="G10" s="11">
         <v>5</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="10" t="s">
         <v>30</v>
       </c>
@@ -1289,11 +1289,11 @@
       <c r="B11" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="10">
         <v>16</v>
       </c>
@@ -1320,19 +1320,19 @@
       <c r="B12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="10">
         <v>18</v>
       </c>
       <c r="G12" s="11">
         <v>5</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="10" t="s">
         <v>30</v>
       </c>
@@ -1382,19 +1382,19 @@
       <c r="B14" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="14"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="14"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="10">
         <v>12</v>
       </c>
       <c r="G14" s="10">
         <v>5</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="10" t="s">
         <v>38</v>
       </c>
@@ -1409,11 +1409,11 @@
       <c r="B15" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="14"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="10">
         <v>8</v>
       </c>
@@ -1440,11 +1440,11 @@
       <c r="B16" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="14"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="14"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="10">
         <v>12</v>
       </c>
@@ -1471,19 +1471,19 @@
       <c r="B17" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="14"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="14"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="10">
         <v>14</v>
       </c>
       <c r="G17" s="10">
         <v>5</v>
       </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="10" t="s">
         <v>38</v>
       </c>
@@ -1498,11 +1498,11 @@
       <c r="B18" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="15"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="10">
         <v>18</v>
       </c>
@@ -1570,7 +1570,7 @@
       <c r="D20" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="10">
         <v>15</v>
       </c>
@@ -1667,11 +1667,11 @@
       <c r="B23" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="15"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="10">
         <v>12</v>
       </c>
@@ -4254,6 +4254,15 @@
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="C22:C23"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="H2:H5"/>
@@ -4270,15 +4279,6 @@
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="C22:C23"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4320,27 +4320,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d0daa353-f819-43d1-badf-ce69fea8800d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Fecha_x0020_de_x0020_creaci_x00f3_n xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
-    <TaxCatchAll xmlns="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d" xsi:nil="true"/>
-    <Fechayhora xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
-    <SharedWithUsers xmlns="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010070BFDEA41A5D8B46AA5DA2E2389CBE4E" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e795e02ad45650978a0fdf890fe0930d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d0daa353-f819-43d1-badf-ce69fea8800d" xmlns:ns3="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48ff01d9d7fae54ca8d4846686737c56" ns2:_="" ns3:_="">
     <xsd:import namespace="d0daa353-f819-43d1-badf-ce69fea8800d"/>
@@ -4589,6 +4568,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d0daa353-f819-43d1-badf-ce69fea8800d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Fecha_x0020_de_x0020_creaci_x00f3_n xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
+    <TaxCatchAll xmlns="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d" xsi:nil="true"/>
+    <Fechayhora xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
+    <SharedWithUsers xmlns="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B13CD9-5B3A-4359-83C6-5F1503DA8E45}">
   <ds:schemaRefs>
@@ -4598,17 +4598,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDC8485E-F7FB-4A0F-8E5D-D6AD519E82D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d0daa353-f819-43d1-badf-ce69fea8800d"/>
-    <ds:schemaRef ds:uri="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA6D3669-63FE-437A-A6EE-CBE94B95DAF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4625,4 +4614,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDC8485E-F7FB-4A0F-8E5D-D6AD519E82D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d0daa353-f819-43d1-badf-ce69fea8800d"/>
+    <ds:schemaRef ds:uri="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>